<commit_message>
August 05 2020 by Prasad
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/TestData/TestData.xlsx
+++ b/Demo/src/test/resources/TestData/TestData.xlsx
@@ -2,27 +2,208 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-484725" yWindow="-478950" windowWidth="16875" windowHeight="2310"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="Credentials" sheetId="2" r:id="rId2"/>
+    <sheet name="Email" sheetId="3" r:id="rId3"/>
+    <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
+    <sheet name="Credential" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>LoginPage</t>
+  </si>
+  <si>
+    <t>OrderPage</t>
+  </si>
+  <si>
+    <t>SearchResultPage</t>
+  </si>
+  <si>
+    <t>AddressPage</t>
+  </si>
+  <si>
+    <t>ShippingPage</t>
+  </si>
+  <si>
+    <t>PaymentPage</t>
+  </si>
+  <si>
+    <t>OrderConfirmationPage</t>
+  </si>
+  <si>
+    <t>IndexPage</t>
+  </si>
+  <si>
+    <t>IndexPageTest</t>
+  </si>
+  <si>
+    <t>AccountCreationPage</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>AddToCartPage</t>
+  </si>
+  <si>
+    <t>Pages Classes</t>
+  </si>
+  <si>
+    <t>TestClasses</t>
+  </si>
+  <si>
+    <t>LoginPageTest</t>
+  </si>
+  <si>
+    <t>HomePageTest</t>
+  </si>
+  <si>
+    <t>AccountCreationTest</t>
+  </si>
+  <si>
+    <t>SearchResultPageTest</t>
+  </si>
+  <si>
+    <t>AddToCartPageTest</t>
+  </si>
+  <si>
+    <t>OrderPageTest</t>
+  </si>
+  <si>
+    <t>EndToEndTest</t>
+  </si>
+  <si>
+    <t>productAvailabilityTest</t>
+  </si>
+  <si>
+    <t>addToCartTest</t>
+  </si>
+  <si>
+    <t>priceTest</t>
+  </si>
+  <si>
+    <t>endToEndTest</t>
+  </si>
+  <si>
+    <t>myStoreLogoTest
+myStoreTitle</t>
+  </si>
+  <si>
+    <t>wishListTest
+orderHistoryandDetailsTest</t>
+  </si>
+  <si>
+    <t>loginTest</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Logo should be present
+Title should match with expected value</t>
+  </si>
+  <si>
+    <t>User should be able to login</t>
+  </si>
+  <si>
+    <t>WishList should be displayed
+OderHistory should be displayed</t>
+  </si>
+  <si>
+    <t>User should be navigate to account creation page</t>
+  </si>
+  <si>
+    <t>Search the product and product should be displayed</t>
+  </si>
+  <si>
+    <t>User should be able to add the product in the cart</t>
+  </si>
+  <si>
+    <t>Validate the Price on Order Page</t>
+  </si>
+  <si>
+    <t>User should be able to order the product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Store Application - </t>
+  </si>
+  <si>
+    <t>OrderSummary</t>
+  </si>
+  <si>
+    <t>createAccountPageTest</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>Sanity</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Sanity, Smoke</t>
+  </si>
+  <si>
+    <t>Regression, Sanity</t>
+  </si>
+  <si>
+    <t>Smoke
+Smoke</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin@xyz.com</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>t-shirt</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ghfsdtyfg@gmail.com</t>
+  </si>
   <si>
     <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
   </si>
   <si>
     <t>prasad@zenwork.com</t>
@@ -35,8 +216,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -51,15 +240,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -67,17 +268,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -373,32 +665,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="7">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -408,28 +1091,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Prasad Commit @08:07 PM 08 August 2020
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/TestData/TestData.xlsx
+++ b/Demo/src/test/resources/TestData/TestData.xlsx
@@ -213,66 +213,9 @@
     <t>Prasad@123</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SSN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FirstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MiddleName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BusinessName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Suffix</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Line2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PayerCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> State </t>
-  </si>
-  <si>
-    <t>Zipcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CheckheretoForeignAddress</t>
-  </si>
-  <si>
     <t xml:space="preserve"> phone</t>
   </si>
   <si>
-    <t xml:space="preserve"> Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WithholdingORTaxStateId</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ClientID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LastFiling</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
@@ -292,6 +235,63 @@
   </si>
   <si>
     <t>United State Of America</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ein</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ssn</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>middlename</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> businessname</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> address</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> suffix</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> line2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> city</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> state </t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> checkheretoforeignaddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> email</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> withholdingortaxstateId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lastfiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clientid</t>
   </si>
 </sst>
 </file>
@@ -1179,101 +1179,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="18" max="18" width="30.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" t="s">
-        <v>77</v>
-      </c>
       <c r="Q1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="R1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="S1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="T1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>889574637</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="M2">
         <v>35010</v>
       </c>
       <c r="N2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="P2">
         <v>123456790</v>

</xml_diff>

<commit_message>
Prasad Commit 2 @11:58 AM 10 August 2020
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/TestData/TestData.xlsx
+++ b/Demo/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -464,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1192,20 +1195,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="14" max="14" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="14"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11" style="14" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C1" t="s">
@@ -1226,7 +1243,7 @@
       <c r="H1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="14" t="s">
         <v>82</v>
       </c>
       <c r="J1" t="s">
@@ -1235,7 +1252,7 @@
       <c r="K1" t="s">
         <v>84</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="14" t="s">
         <v>62</v>
       </c>
       <c r="M1" t="s">
@@ -1247,7 +1264,7 @@
       <c r="O1" t="s">
         <v>87</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="14" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1255,7 +1272,7 @@
       <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="14">
         <v>889574637</v>
       </c>
       <c r="C2" t="s">
@@ -1273,19 +1290,19 @@
       <c r="H2" t="s">
         <v>68</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="14">
         <v>35010</v>
       </c>
       <c r="J2" t="s">
         <v>69</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="14">
         <v>123456790</v>
       </c>
       <c r="M2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="14">
         <v>12345</v>
       </c>
     </row>
@@ -1301,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Prasad commit August 13 2020 10:50 PM
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/TestData/TestData.xlsx
+++ b/Demo/src/test/resources/TestData/TestData.xlsx
@@ -446,7 +446,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -480,6 +480,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1207,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15"/>
@@ -1294,41 +1299,42 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
+    <row r="2" spans="1:20" s="15" customFormat="1">
+      <c r="A2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="16">
         <v>889574637</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="16">
         <v>35010</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="16">
         <v>123456790</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="16">
         <v>12345</v>
       </c>
     </row>
@@ -1337,6 +1343,7 @@
     <hyperlink ref="Q2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
OCT 10 20 2020
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/TestData/TestData.xlsx
+++ b/Demo/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -13,15 +13,16 @@
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
     <sheet name="Credential" sheetId="7" r:id="rId6"/>
-    <sheet name="AddPayerein" sheetId="8" r:id="rId7"/>
+    <sheet name="AddPayereinTest" sheetId="8" r:id="rId7"/>
     <sheet name="AddPayerssn" sheetId="9" r:id="rId8"/>
+    <sheet name="AddPayerein" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="113">
   <si>
     <t>TestCases</t>
   </si>
@@ -317,6 +318,54 @@
   </si>
   <si>
     <t>LastName</t>
+  </si>
+  <si>
+    <t>einTIN</t>
+  </si>
+  <si>
+    <t>businessname</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>suffix</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>withholdingortaxstateid</t>
+  </si>
+  <si>
+    <t>clientid</t>
+  </si>
+  <si>
+    <t>PrasadTestAA01</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>prasad@test1.com</t>
+  </si>
+  <si>
+    <t>R123456789</t>
   </si>
 </sst>
 </file>
@@ -471,6 +520,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -480,11 +534,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -827,13 +876,13 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
@@ -1210,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15"/>
@@ -1228,16 +1277,15 @@
     <col min="11" max="11" width="5.85546875" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" style="11"/>
-    <col min="14" max="14" width="22.42578125" customWidth="1"/>
-    <col min="15" max="15" width="25.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="11" style="11" customWidth="1"/>
     <col min="17" max="17" width="21.140625" customWidth="1"/>
     <col min="18" max="18" width="23.140625" customWidth="1"/>
-    <col min="19" max="19" width="9" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="11"/>
+    <col min="19" max="19" width="15.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -1292,49 +1340,46 @@
       <c r="R1" t="s">
         <v>86</v>
       </c>
-      <c r="S1" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="15" customFormat="1">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:19" s="12" customFormat="1">
+      <c r="A2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="13">
         <v>889574637</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="13">
         <v>35010</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="13">
         <v>123456790</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="16">
+      <c r="S2" s="13">
         <v>12345</v>
       </c>
     </row>
@@ -1352,7 +1397,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1472,4 +1517,111 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>450593832</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2">
+        <v>35010</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2">
+        <v>1234567890</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 1:25 AM 12/18/2020
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/TestData/TestData.xlsx
+++ b/Demo/src/test/resources/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
   <si>
     <t>TestCases</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>R123456789</t>
+  </si>
+  <si>
+    <t>United States of America</t>
   </si>
 </sst>
 </file>
@@ -1524,14 +1527,14 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" customWidth="1"/>
   </cols>
@@ -1577,51 +1580,49 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
+    <row r="2" spans="1:13" s="12" customFormat="1">
+      <c r="A2" s="12">
         <v>450593832</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="12">
         <v>35010</v>
       </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="12">
         <v>1234567890</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="12">
         <v>12345</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>